<commit_message>
prepping for making public
</commit_message>
<xml_diff>
--- a/roots-messy.xlsx
+++ b/roots-messy.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="101">
   <si>
     <t>worms</t>
   </si>
@@ -313,6 +313,15 @@
   </si>
   <si>
     <t>absent or present</t>
+  </si>
+  <si>
+    <t>Data from Cameron EK, Cahill JF Jr, Bayne EM (2014) Root Foraging Influences Plant Growth Responses to Earthworm Foraging. PLoS ONE 9(9): e108873. doi:10.1371/journal.pone.0108873</t>
+  </si>
+  <si>
+    <t>Original data is available at https://era.library.ualberta.ca/files/z029p5988#.WIKrJZJVeAA</t>
+  </si>
+  <si>
+    <t>The data in this spreadsheet has had flaws introduced for educational purposes.</t>
   </si>
 </sst>
 </file>
@@ -391,8 +400,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -433,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -449,6 +462,8 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -464,6 +479,8 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -766,120 +783,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I74"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="4" spans="1:9">
-      <c r="A4" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2.8765000000000001</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3.4365999999999999</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1.0565739999999999</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1.234483</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" s="2">
-        <v>2.7765</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1.2232000000000001</v>
-      </c>
-      <c r="G7" s="2">
-        <v>10.79</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1.021191</v>
-      </c>
-      <c r="I7" s="2">
-        <v>0.20147029999999999</v>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>86</v>
@@ -888,27 +862,27 @@
         <v>92</v>
       </c>
       <c r="E8" s="2">
-        <v>2.1311</v>
+        <v>2.8765000000000001</v>
       </c>
       <c r="F8" s="2">
-        <v>1.5024</v>
-      </c>
-      <c r="G8" s="2">
-        <v>28.23</v>
+        <v>3.4365999999999999</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="H8" s="2">
-        <v>0.75663820000000004</v>
+        <v>1.0565739999999999</v>
       </c>
       <c r="I8" s="2">
-        <v>0.40706379999999998</v>
+        <v>1.234483</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -917,143 +891,143 @@
         <v>92</v>
       </c>
       <c r="E9" s="2">
-        <v>2.6196999999999999</v>
+        <v>2.7765</v>
       </c>
       <c r="F9" s="2">
-        <v>0.57779999999999998</v>
+        <v>1.2232000000000001</v>
       </c>
       <c r="G9" s="2">
-        <v>10.15</v>
+        <v>10.79</v>
       </c>
       <c r="H9" s="2">
-        <v>0.96305980000000002</v>
+        <v>1.021191</v>
       </c>
       <c r="I9" s="2">
-        <v>-0.54852749999999995</v>
+        <v>0.20147029999999999</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E10" s="2">
-        <v>2.9426000000000001</v>
+        <v>2.1311</v>
       </c>
       <c r="F10" s="2">
-        <v>1.0198</v>
+        <v>1.5024</v>
       </c>
       <c r="G10" s="2">
-        <v>36.4</v>
+        <v>28.23</v>
       </c>
       <c r="H10" s="2">
-        <v>1.0792930000000001</v>
+        <v>0.75663820000000004</v>
       </c>
       <c r="I10" s="2">
-        <v>1.9606499999999999E-2</v>
+        <v>0.40706379999999998</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E11" s="2">
-        <v>2.7829000000000002</v>
+        <v>2.6196999999999999</v>
       </c>
       <c r="F11" s="2">
-        <v>3.3031000000000001</v>
+        <v>0.57779999999999998</v>
       </c>
       <c r="G11" s="2">
-        <v>33.270000000000003</v>
+        <v>10.15</v>
       </c>
       <c r="H11" s="2">
-        <v>1.0234939999999999</v>
+        <v>0.96305980000000002</v>
       </c>
       <c r="I11" s="2">
-        <v>1.194861</v>
+        <v>-0.54852749999999995</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>4</v>
+        <v>82</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E12" s="2">
-        <v>1.8328</v>
+        <v>2.9426000000000001</v>
       </c>
       <c r="F12" s="2">
-        <v>1.0266999999999999</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>84</v>
+        <v>1.0198</v>
+      </c>
+      <c r="G12" s="2">
+        <v>36.4</v>
       </c>
       <c r="H12" s="2">
-        <v>0.60584490000000002</v>
+        <v>1.0792930000000001</v>
       </c>
       <c r="I12" s="2">
-        <v>2.63498E-2</v>
+        <v>1.9606499999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E13" s="2">
-        <v>2.4952000000000001</v>
+        <v>2.7829000000000002</v>
       </c>
       <c r="F13" s="2">
-        <v>1.1754</v>
+        <v>3.3031000000000001</v>
       </c>
       <c r="G13" s="2">
-        <v>12.43</v>
+        <v>33.270000000000003</v>
       </c>
       <c r="H13" s="2">
-        <v>0.91436890000000004</v>
+        <v>1.0234939999999999</v>
       </c>
       <c r="I13" s="2">
-        <v>0.16160849999999999</v>
+        <v>1.194861</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>4</v>
@@ -1062,27 +1036,27 @@
         <v>92</v>
       </c>
       <c r="E14" s="2">
-        <v>2.367</v>
+        <v>1.8328</v>
       </c>
       <c r="F14" s="2">
-        <v>0.89139999999999997</v>
-      </c>
-      <c r="G14" s="2">
-        <v>9.32</v>
+        <v>1.0266999999999999</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="H14" s="2">
-        <v>0.86162329999999998</v>
+        <v>0.60584490000000002</v>
       </c>
       <c r="I14" s="2">
-        <v>-0.11496199999999999</v>
+        <v>2.63498E-2</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>4</v>
@@ -1091,56 +1065,56 @@
         <v>92</v>
       </c>
       <c r="E15" s="2">
-        <v>2.1198000000000001</v>
+        <v>2.4952000000000001</v>
       </c>
       <c r="F15" s="2">
-        <v>0.96330000000000005</v>
+        <v>1.1754</v>
       </c>
       <c r="G15" s="2">
-        <v>10.09</v>
+        <v>12.43</v>
       </c>
       <c r="H15" s="2">
-        <v>0.75132180000000004</v>
+        <v>0.91436890000000004</v>
       </c>
       <c r="I15" s="2">
-        <v>-3.7390399999999997E-2</v>
+        <v>0.16160849999999999</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E16" s="2">
-        <v>2.7406000000000001</v>
+        <v>2.367</v>
       </c>
       <c r="F16" s="2">
-        <v>2.3397999999999999</v>
+        <v>0.89139999999999997</v>
       </c>
       <c r="G16" s="2">
-        <v>31.56</v>
+        <v>9.32</v>
       </c>
       <c r="H16" s="2">
-        <v>1.0081770000000001</v>
+        <v>0.86162329999999998</v>
       </c>
       <c r="I16" s="2">
-        <v>0.85006539999999997</v>
+        <v>-0.11496199999999999</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>4</v>
@@ -1149,27 +1123,27 @@
         <v>92</v>
       </c>
       <c r="E17" s="2">
-        <v>1.8035000000000001</v>
+        <v>2.1198000000000001</v>
       </c>
       <c r="F17" s="2">
-        <v>1.0213000000000001</v>
+        <v>0.96330000000000005</v>
       </c>
       <c r="G17" s="2">
-        <v>12.14</v>
+        <v>10.09</v>
       </c>
       <c r="H17" s="2">
-        <v>0.58972919999999995</v>
+        <v>0.75132180000000004</v>
       </c>
       <c r="I17" s="2">
-        <v>2.1076299999999999E-2</v>
+        <v>-3.7390399999999997E-2</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>3</v>
@@ -1178,85 +1152,85 @@
         <v>92</v>
       </c>
       <c r="E18" s="2">
-        <v>1.8512999999999999</v>
+        <v>2.7406000000000001</v>
       </c>
       <c r="F18" s="2">
-        <v>1.5573999999999999</v>
+        <v>2.3397999999999999</v>
       </c>
       <c r="G18" s="2">
-        <v>35.4</v>
+        <v>31.56</v>
       </c>
       <c r="H18" s="2">
-        <v>0.61588810000000005</v>
+        <v>1.0081770000000001</v>
       </c>
       <c r="I18" s="2">
-        <v>0.44301780000000002</v>
+        <v>0.85006539999999997</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E19" s="2">
-        <v>2.9889000000000001</v>
+        <v>1.8035000000000001</v>
       </c>
       <c r="F19" s="2">
-        <v>1.7602</v>
+        <v>1.0213000000000001</v>
       </c>
       <c r="G19" s="2">
-        <v>33.020000000000003</v>
+        <v>12.14</v>
       </c>
       <c r="H19" s="2">
-        <v>1.094905</v>
+        <v>0.58972919999999995</v>
       </c>
       <c r="I19" s="2">
-        <v>0.56542749999999997</v>
+        <v>2.1076299999999999E-2</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="2" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E20" s="2">
-        <v>1.9426000000000001</v>
+        <v>1.8512999999999999</v>
       </c>
       <c r="F20" s="2">
-        <v>1.6464000000000001</v>
+        <v>1.5573999999999999</v>
       </c>
       <c r="G20" s="2">
-        <v>8.02</v>
+        <v>35.4</v>
       </c>
       <c r="H20" s="2">
-        <v>0.66402729999999999</v>
+        <v>0.61588810000000005</v>
       </c>
       <c r="I20" s="2">
-        <v>0.49859110000000001</v>
+        <v>0.44301780000000002</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
@@ -1265,19 +1239,19 @@
         <v>92</v>
       </c>
       <c r="E21" s="2">
-        <v>3.2088000000000001</v>
+        <v>2.9889000000000001</v>
       </c>
       <c r="F21" s="2">
-        <v>3.7187000000000001</v>
+        <v>1.7602</v>
       </c>
       <c r="G21" s="2">
-        <v>30.37</v>
+        <v>33.020000000000003</v>
       </c>
       <c r="H21" s="2">
-        <v>1.165897</v>
+        <v>1.094905</v>
       </c>
       <c r="I21" s="2">
-        <v>1.313374</v>
+        <v>0.56542749999999997</v>
       </c>
     </row>
     <row r="22" spans="1:9">
@@ -1285,36 +1259,36 @@
         <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E22" s="2">
-        <v>1.6543000000000001</v>
+        <v>1.9426000000000001</v>
       </c>
       <c r="F22" s="2">
-        <v>2.3687999999999998</v>
+        <v>1.6464000000000001</v>
       </c>
       <c r="G22" s="2">
-        <v>34.119999999999997</v>
+        <v>8.02</v>
       </c>
       <c r="H22" s="2">
-        <v>0.50337790000000004</v>
+        <v>0.66402729999999999</v>
       </c>
       <c r="I22" s="2">
-        <v>0.86238349999999997</v>
+        <v>0.49859110000000001</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>3</v>
@@ -1323,27 +1297,27 @@
         <v>92</v>
       </c>
       <c r="E23" s="2">
-        <v>2.9222999999999999</v>
+        <v>3.2088000000000001</v>
       </c>
       <c r="F23" s="2">
-        <v>2.1631999999999998</v>
+        <v>3.7187000000000001</v>
       </c>
       <c r="G23" s="2">
-        <v>32.14</v>
+        <v>30.37</v>
       </c>
       <c r="H23" s="2">
-        <v>1.072371</v>
+        <v>1.165897</v>
       </c>
       <c r="I23" s="2">
-        <v>0.77158859999999996</v>
+        <v>1.313374</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="2" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>3</v>
@@ -1352,114 +1326,114 @@
         <v>92</v>
       </c>
       <c r="E24" s="2">
-        <v>3.6852999999999998</v>
+        <v>1.6543000000000001</v>
       </c>
       <c r="F24" s="2">
-        <v>3.0834000000000001</v>
+        <v>2.3687999999999998</v>
       </c>
       <c r="G24" s="2">
-        <v>41.91</v>
+        <v>34.119999999999997</v>
       </c>
       <c r="H24" s="2">
-        <v>1.304352</v>
+        <v>0.50337790000000004</v>
       </c>
       <c r="I24" s="2">
-        <v>1.1260330000000001</v>
+        <v>0.86238349999999997</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E25" s="2">
-        <v>1.6469</v>
+        <v>2.9222999999999999</v>
       </c>
       <c r="F25" s="2">
-        <v>0.75160000000000005</v>
+        <v>2.1631999999999998</v>
       </c>
       <c r="G25" s="2">
-        <v>7.83</v>
+        <v>32.14</v>
       </c>
       <c r="H25" s="2">
-        <v>0.49889480000000003</v>
+        <v>1.072371</v>
       </c>
       <c r="I25" s="2">
-        <v>-0.285551</v>
+        <v>0.77158859999999996</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E26" s="2">
-        <v>1.8478000000000001</v>
+        <v>3.6852999999999998</v>
       </c>
       <c r="F26" s="2">
-        <v>0.73670000000000002</v>
+        <v>3.0834000000000001</v>
       </c>
       <c r="G26" s="2">
-        <v>9.93</v>
+        <v>41.91</v>
       </c>
       <c r="H26" s="2">
-        <v>0.61399570000000003</v>
+        <v>1.304352</v>
       </c>
       <c r="I26" s="2">
-        <v>-0.30557450000000003</v>
+        <v>1.1260330000000001</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E27" s="2">
-        <v>5.2866999999999997</v>
+        <v>1.6469</v>
       </c>
       <c r="F27" s="2">
-        <v>2.7094</v>
+        <v>0.75160000000000005</v>
       </c>
       <c r="G27" s="2">
-        <v>41.79</v>
+        <v>7.83</v>
       </c>
       <c r="H27" s="2">
-        <v>1.6651940000000001</v>
+        <v>0.49889480000000003</v>
       </c>
       <c r="I27" s="2">
-        <v>0.99672720000000004</v>
+        <v>-0.285551</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>4</v>
@@ -1468,172 +1442,172 @@
         <v>92</v>
       </c>
       <c r="E28" s="2">
-        <v>1.3976999999999999</v>
+        <v>1.8478000000000001</v>
       </c>
       <c r="F28" s="2">
-        <v>0.74880000000000002</v>
+        <v>0.73670000000000002</v>
       </c>
       <c r="G28" s="2">
-        <v>9.23</v>
+        <v>9.93</v>
       </c>
       <c r="H28" s="2">
-        <v>0.33482800000000001</v>
+        <v>0.61399570000000003</v>
       </c>
       <c r="I28" s="2">
-        <v>-0.28928340000000002</v>
+        <v>-0.30557450000000003</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="2" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E29" s="2">
-        <v>3.4605999999999999</v>
+        <v>5.2866999999999997</v>
       </c>
       <c r="F29" s="2">
-        <v>1.4091</v>
+        <v>2.7094</v>
       </c>
       <c r="G29" s="2">
-        <v>9.26</v>
+        <v>41.79</v>
       </c>
       <c r="H29" s="2">
-        <v>1.2414419999999999</v>
+        <v>1.6651940000000001</v>
       </c>
       <c r="I29" s="2">
-        <v>0.34295120000000001</v>
+        <v>0.99672720000000004</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="2" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E30" s="2">
-        <v>2.8494000000000002</v>
+        <v>1.3976999999999999</v>
       </c>
       <c r="F30" s="2">
-        <v>2.0350999999999999</v>
+        <v>0.74880000000000002</v>
       </c>
       <c r="G30" s="2">
-        <v>37.51</v>
+        <v>9.23</v>
       </c>
       <c r="H30" s="2">
-        <v>1.0471079999999999</v>
+        <v>0.33482800000000001</v>
       </c>
       <c r="I30" s="2">
-        <v>0.71054490000000003</v>
+        <v>-0.28928340000000002</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="2" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="2">
-        <v>3.6785999999999999</v>
+        <v>3.4605999999999999</v>
       </c>
       <c r="F31" s="2">
-        <v>3.0516000000000001</v>
+        <v>1.4091</v>
       </c>
       <c r="G31" s="2">
-        <v>36.590000000000003</v>
+        <v>9.26</v>
       </c>
       <c r="H31" s="2">
-        <v>1.302532</v>
+        <v>1.2414419999999999</v>
       </c>
       <c r="I31" s="2">
-        <v>1.115666</v>
+        <v>0.34295120000000001</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E32" s="2">
-        <v>1.9676</v>
+        <v>2.8494000000000002</v>
       </c>
       <c r="F32" s="2">
-        <v>0.7913</v>
+        <v>2.0350999999999999</v>
       </c>
       <c r="G32" s="2">
-        <v>10.75</v>
+        <v>37.51</v>
       </c>
       <c r="H32" s="2">
-        <v>0.67681449999999999</v>
+        <v>1.0471079999999999</v>
       </c>
       <c r="I32" s="2">
-        <v>-0.23407810000000001</v>
+        <v>0.71054490000000003</v>
       </c>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>92</v>
       </c>
       <c r="E33" s="2">
-        <v>2.0044</v>
+        <v>3.6785999999999999</v>
       </c>
       <c r="F33" s="2">
-        <v>0.77849999999999997</v>
+        <v>3.0516000000000001</v>
       </c>
       <c r="G33" s="2">
-        <v>12.6</v>
+        <v>36.590000000000003</v>
       </c>
       <c r="H33" s="2">
-        <v>0.69534470000000004</v>
+        <v>1.302532</v>
       </c>
       <c r="I33" s="2">
-        <v>-0.25038630000000001</v>
+        <v>1.115666</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="2" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>4</v>
@@ -1642,172 +1616,172 @@
         <v>92</v>
       </c>
       <c r="E34" s="2">
-        <v>1.5553999999999999</v>
+        <v>1.9676</v>
       </c>
       <c r="F34" s="2">
-        <v>0.19350000000000001</v>
+        <v>0.7913</v>
       </c>
       <c r="G34" s="2">
-        <v>9.69</v>
+        <v>10.75</v>
       </c>
       <c r="H34" s="2">
-        <v>0.44173279999999998</v>
+        <v>0.67681449999999999</v>
       </c>
       <c r="I34" s="2">
-        <v>-1.6424780000000001</v>
+        <v>-0.23407810000000001</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="2" t="s">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E35" s="2">
-        <v>1.875</v>
+        <v>2.0044</v>
       </c>
       <c r="F35" s="2">
-        <v>1.2040999999999999</v>
+        <v>0.77849999999999997</v>
       </c>
       <c r="G35" s="2">
-        <v>11.15</v>
+        <v>12.6</v>
       </c>
       <c r="H35" s="2">
-        <v>0.62860859999999996</v>
+        <v>0.69534470000000004</v>
       </c>
       <c r="I35" s="2">
-        <v>0.18573239999999999</v>
+        <v>-0.25038630000000001</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E36" s="2">
-        <v>3.7551999999999999</v>
+        <v>1.5553999999999999</v>
       </c>
       <c r="F36" s="2">
-        <v>3.8266</v>
+        <v>0.19350000000000001</v>
       </c>
       <c r="G36" s="2">
-        <v>29.88</v>
+        <v>9.69</v>
       </c>
       <c r="H36" s="2">
-        <v>1.323142</v>
+        <v>0.44173279999999998</v>
       </c>
       <c r="I36" s="2">
-        <v>1.341977</v>
+        <v>-1.6424780000000001</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="2" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>90</v>
       </c>
       <c r="E37" s="2">
-        <v>3.8016000000000001</v>
+        <v>1.875</v>
       </c>
       <c r="F37" s="2">
-        <v>2.7174999999999998</v>
+        <v>1.2040999999999999</v>
       </c>
       <c r="G37" s="2">
-        <v>40.49</v>
+        <v>11.15</v>
       </c>
       <c r="H37" s="2">
-        <v>1.3354220000000001</v>
+        <v>0.62860859999999996</v>
       </c>
       <c r="I37" s="2">
-        <v>0.9997123</v>
+        <v>0.18573239999999999</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E38" s="2">
-        <v>2.8422000000000001</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>85</v>
+        <v>3.7551999999999999</v>
+      </c>
+      <c r="F38" s="2">
+        <v>3.8266</v>
       </c>
       <c r="G38" s="2">
-        <v>39.47</v>
+        <v>29.88</v>
       </c>
       <c r="H38" s="2">
-        <v>1.044578</v>
+        <v>1.323142</v>
       </c>
       <c r="I38" s="2">
-        <v>0.79755220000000004</v>
+        <v>1.341977</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E39" s="2">
-        <v>2.5106000000000002</v>
+        <v>3.8016000000000001</v>
       </c>
       <c r="F39" s="2">
-        <v>3.4729000000000001</v>
+        <v>2.7174999999999998</v>
       </c>
       <c r="G39" s="2">
-        <v>31.56</v>
+        <v>40.49</v>
       </c>
       <c r="H39" s="2">
-        <v>0.92052179999999995</v>
+        <v>1.3354220000000001</v>
       </c>
       <c r="I39" s="2">
-        <v>1.24499</v>
+        <v>0.9997123</v>
       </c>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>3</v>
@@ -1816,27 +1790,27 @@
         <v>91</v>
       </c>
       <c r="E40" s="2">
-        <v>2.5466000000000002</v>
-      </c>
-      <c r="F40" s="2">
-        <v>3.5743999999999998</v>
+        <v>2.8422000000000001</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="G40" s="2">
-        <v>39.630000000000003</v>
+        <v>39.47</v>
       </c>
       <c r="H40" s="2">
-        <v>0.93475920000000001</v>
+        <v>1.044578</v>
       </c>
       <c r="I40" s="2">
-        <v>1.2737970000000001</v>
+        <v>0.79755220000000004</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="2" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>3</v>
@@ -1845,143 +1819,143 @@
         <v>91</v>
       </c>
       <c r="E41" s="2">
-        <v>5.9150999999999998</v>
+        <v>2.5106000000000002</v>
       </c>
       <c r="F41" s="2">
-        <v>2.5878999999999999</v>
+        <v>3.4729000000000001</v>
       </c>
       <c r="G41" s="2">
-        <v>36.83</v>
+        <v>31.56</v>
       </c>
       <c r="H41" s="2">
-        <v>1.7775080000000001</v>
+        <v>0.92052179999999995</v>
       </c>
       <c r="I41" s="2">
-        <v>0.95084670000000004</v>
+        <v>1.24499</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E42" s="2">
-        <v>1.5006999999999999</v>
+        <v>2.5466000000000002</v>
       </c>
       <c r="F42" s="2">
-        <v>0.36320000000000002</v>
+        <v>3.5743999999999998</v>
       </c>
       <c r="G42" s="2">
-        <v>10.73</v>
+        <v>39.630000000000003</v>
       </c>
       <c r="H42" s="2">
-        <v>0.40593170000000001</v>
+        <v>0.93475920000000001</v>
       </c>
       <c r="I42" s="2">
-        <v>-1.012802</v>
+        <v>1.2737970000000001</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" s="2" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E43" s="2">
-        <v>0.96460000000000001</v>
+        <v>5.9150999999999998</v>
       </c>
       <c r="F43" s="2">
-        <v>0.25659999999999999</v>
+        <v>2.5878999999999999</v>
       </c>
       <c r="G43" s="2">
-        <v>10.37</v>
+        <v>36.83</v>
       </c>
       <c r="H43" s="2">
-        <v>-3.6041700000000003E-2</v>
+        <v>1.7775080000000001</v>
       </c>
       <c r="I43" s="2">
-        <v>-1.3602369999999999</v>
+        <v>0.95084670000000004</v>
       </c>
     </row>
     <row r="44" spans="1:9">
       <c r="A44" s="2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D44" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E44" s="2">
-        <v>2.3542000000000001</v>
+        <v>1.5006999999999999</v>
       </c>
       <c r="F44" s="2">
-        <v>2.6048</v>
+        <v>0.36320000000000002</v>
       </c>
       <c r="G44" s="2">
-        <v>33.78</v>
+        <v>10.73</v>
       </c>
       <c r="H44" s="2">
-        <v>0.85620090000000004</v>
+        <v>0.40593170000000001</v>
       </c>
       <c r="I44" s="2">
-        <v>0.95735590000000004</v>
+        <v>-1.012802</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="2" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E45" s="2">
-        <v>2.2755999999999998</v>
+        <v>0.96460000000000001</v>
       </c>
       <c r="F45" s="2">
-        <v>2.2138</v>
+        <v>0.25659999999999999</v>
       </c>
       <c r="G45" s="2">
-        <v>29.49</v>
+        <v>10.37</v>
       </c>
       <c r="H45" s="2">
-        <v>0.82224379999999997</v>
+        <v>-3.6041700000000003E-2</v>
       </c>
       <c r="I45" s="2">
-        <v>0.79471049999999999</v>
+        <v>-1.3602369999999999</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" s="2" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>3</v>
@@ -1990,27 +1964,27 @@
         <v>91</v>
       </c>
       <c r="E46" s="2">
-        <v>4.4924999999999997</v>
+        <v>2.3542000000000001</v>
       </c>
       <c r="F46" s="2">
-        <v>3.1541999999999999</v>
+        <v>2.6048</v>
       </c>
       <c r="G46" s="2">
-        <v>41.52</v>
+        <v>33.78</v>
       </c>
       <c r="H46" s="2">
-        <v>1.5024090000000001</v>
+        <v>0.85620090000000004</v>
       </c>
       <c r="I46" s="2">
-        <v>1.1487350000000001</v>
+        <v>0.95735590000000004</v>
       </c>
     </row>
     <row r="47" spans="1:9">
       <c r="A47" s="2" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>3</v>
@@ -2019,85 +1993,85 @@
         <v>91</v>
       </c>
       <c r="E47" s="2">
-        <v>2.8597999999999999</v>
+        <v>2.2755999999999998</v>
       </c>
       <c r="F47" s="2">
-        <v>1.7201</v>
+        <v>2.2138</v>
       </c>
       <c r="G47" s="2">
-        <v>33.97</v>
+        <v>29.49</v>
       </c>
       <c r="H47" s="2">
-        <v>1.0507519999999999</v>
+        <v>0.82224379999999997</v>
       </c>
       <c r="I47" s="2">
-        <v>0.54238249999999999</v>
+        <v>0.79471049999999999</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E48" s="2">
-        <v>1.6240000000000001</v>
+        <v>4.4924999999999997</v>
       </c>
       <c r="F48" s="2">
-        <v>0.436</v>
+        <v>3.1541999999999999</v>
       </c>
       <c r="G48" s="2">
-        <v>10.38</v>
+        <v>41.52</v>
       </c>
       <c r="H48" s="2">
-        <v>0.4848922</v>
+        <v>1.5024090000000001</v>
       </c>
       <c r="I48" s="2">
-        <v>-0.83011310000000005</v>
+        <v>1.1487350000000001</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D49" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E49" s="2">
-        <v>1.9899</v>
+        <v>2.8597999999999999</v>
       </c>
       <c r="F49" s="2">
-        <v>1.3382000000000001</v>
+        <v>1.7201</v>
       </c>
       <c r="G49" s="2">
-        <v>11.11</v>
+        <v>33.97</v>
       </c>
       <c r="H49" s="2">
-        <v>0.68808440000000004</v>
+        <v>1.0507519999999999</v>
       </c>
       <c r="I49" s="2">
-        <v>0.29132540000000001</v>
+        <v>0.54238249999999999</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="2" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>4</v>
@@ -2106,27 +2080,27 @@
         <v>91</v>
       </c>
       <c r="E50" s="2">
-        <v>1.4173</v>
+        <v>1.6240000000000001</v>
       </c>
       <c r="F50" s="2">
-        <v>1.0014000000000001</v>
+        <v>0.436</v>
       </c>
       <c r="G50" s="2">
-        <v>8.4</v>
+        <v>10.38</v>
       </c>
       <c r="H50" s="2">
-        <v>0.3487536</v>
+        <v>0.4848922</v>
       </c>
       <c r="I50" s="2">
-        <v>1.3990000000000001E-3</v>
+        <v>-0.83011310000000005</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>4</v>
@@ -2135,56 +2109,56 @@
         <v>91</v>
       </c>
       <c r="E51" s="2">
-        <v>1.8926000000000001</v>
+        <v>1.9899</v>
       </c>
       <c r="F51" s="2">
-        <v>1.3085</v>
+        <v>1.3382000000000001</v>
       </c>
       <c r="G51" s="2">
-        <v>6.81</v>
+        <v>11.11</v>
       </c>
       <c r="H51" s="2">
-        <v>0.63795159999999995</v>
+        <v>0.68808440000000004</v>
       </c>
       <c r="I51" s="2">
-        <v>0.2688815</v>
+        <v>0.29132540000000001</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="2" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D52" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E52" s="2">
-        <v>4.5467000000000004</v>
+        <v>1.4173</v>
       </c>
       <c r="F52" s="2">
-        <v>0.93579999999999997</v>
+        <v>1.0014000000000001</v>
       </c>
       <c r="G52" s="2">
-        <v>38.020000000000003</v>
+        <v>8.4</v>
       </c>
       <c r="H52" s="2">
-        <v>1.514402</v>
+        <v>0.3487536</v>
       </c>
       <c r="I52" s="2">
-        <v>-6.6353499999999996E-2</v>
+        <v>1.3990000000000001E-3</v>
       </c>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="2" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C53" s="2" t="s">
         <v>4</v>
@@ -2193,56 +2167,56 @@
         <v>91</v>
       </c>
       <c r="E53" s="2">
-        <v>0.61760000000000004</v>
+        <v>1.8926000000000001</v>
       </c>
       <c r="F53" s="2">
-        <v>0.32919999999999999</v>
+        <v>1.3085</v>
       </c>
       <c r="G53" s="2">
-        <v>8.73</v>
+        <v>6.81</v>
       </c>
       <c r="H53" s="2">
-        <v>-0.48191430000000002</v>
+        <v>0.63795159999999995</v>
       </c>
       <c r="I53" s="2">
-        <v>-1.1110899999999999</v>
+        <v>0.2688815</v>
       </c>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="2" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>93</v>
+        <v>3</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E54" s="2">
-        <v>0.22170000000000001</v>
+        <v>4.5467000000000004</v>
       </c>
       <c r="F54" s="2">
-        <v>0.1169</v>
+        <v>0.93579999999999997</v>
       </c>
       <c r="G54" s="2">
-        <v>12.02</v>
+        <v>38.020000000000003</v>
       </c>
       <c r="H54" s="2">
-        <v>-1.5064299999999999</v>
+        <v>1.514402</v>
       </c>
       <c r="I54" s="2">
-        <v>-2.146436</v>
+        <v>-6.6353499999999996E-2</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="2" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>4</v>
@@ -2251,56 +2225,56 @@
         <v>91</v>
       </c>
       <c r="E55" s="2">
-        <v>0.69579999999999997</v>
+        <v>0.61760000000000004</v>
       </c>
       <c r="F55" s="2">
-        <v>0.2515</v>
+        <v>0.32919999999999999</v>
       </c>
       <c r="G55" s="2">
-        <v>10.53</v>
+        <v>8.73</v>
       </c>
       <c r="H55" s="2">
-        <v>-0.36269299999999999</v>
+        <v>-0.48191430000000002</v>
       </c>
       <c r="I55" s="2">
-        <v>-1.380312</v>
+        <v>-1.1110899999999999</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="2" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="D56" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="2">
-        <v>2.766</v>
+        <v>0.22170000000000001</v>
       </c>
       <c r="F56" s="2">
-        <v>1.7444</v>
+        <v>0.1169</v>
       </c>
       <c r="G56" s="2">
-        <v>29.14</v>
+        <v>12.02</v>
       </c>
       <c r="H56" s="2">
-        <v>1.0174019999999999</v>
+        <v>-1.5064299999999999</v>
       </c>
       <c r="I56" s="2">
-        <v>0.55641070000000004</v>
+        <v>-2.146436</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="2" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>4</v>
@@ -2309,27 +2283,27 @@
         <v>91</v>
       </c>
       <c r="E57" s="2">
-        <v>1.125</v>
+        <v>0.69579999999999997</v>
       </c>
       <c r="F57" s="2">
-        <v>0.2276</v>
+        <v>0.2515</v>
       </c>
       <c r="G57" s="2">
-        <v>8.31</v>
+        <v>10.53</v>
       </c>
       <c r="H57" s="2">
-        <v>0.117783</v>
+        <v>-0.36269299999999999</v>
       </c>
       <c r="I57" s="2">
-        <v>-1.4801660000000001</v>
+        <v>-1.380312</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="2" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>3</v>
@@ -2338,48 +2312,48 @@
         <v>91</v>
       </c>
       <c r="E58" s="2">
-        <v>3.2810000000000001</v>
+        <v>2.766</v>
       </c>
       <c r="F58" s="2">
-        <v>1.5036</v>
+        <v>1.7444</v>
       </c>
       <c r="G58" s="2">
-        <v>36.53</v>
+        <v>29.14</v>
       </c>
       <c r="H58" s="2">
-        <v>1.188148</v>
+        <v>1.0174019999999999</v>
       </c>
       <c r="I58" s="2">
-        <v>0.40786220000000001</v>
+        <v>0.55641070000000004</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="2" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D59" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E59" s="2">
-        <v>2.8157999999999999</v>
-      </c>
-      <c r="F59" s="2" t="s">
-        <v>83</v>
+        <v>1.125</v>
+      </c>
+      <c r="F59" s="2">
+        <v>0.2276</v>
       </c>
       <c r="G59" s="2">
-        <v>35.92</v>
+        <v>8.31</v>
       </c>
       <c r="H59" s="2">
-        <v>1.0352460000000001</v>
-      </c>
-      <c r="I59" s="2" t="s">
-        <v>85</v>
+        <v>0.117783</v>
+      </c>
+      <c r="I59" s="2">
+        <v>-1.4801660000000001</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2387,63 +2361,65 @@
         <v>20</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D60" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E60" s="2">
-        <v>1.7273000000000001</v>
+        <v>3.2810000000000001</v>
       </c>
       <c r="F60" s="2">
-        <v>0.60680000000000001</v>
+        <v>1.5036</v>
       </c>
       <c r="G60" s="2">
-        <v>8.16</v>
+        <v>36.53</v>
       </c>
       <c r="H60" s="2">
-        <v>0.54655949999999998</v>
+        <v>1.188148</v>
       </c>
       <c r="I60" s="2">
-        <v>-0.499556</v>
+        <v>0.40786220000000001</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D61" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E61" s="2">
-        <v>1.8523000000000001</v>
-      </c>
-      <c r="F61" s="2">
-        <v>0.75090000000000001</v>
-      </c>
-      <c r="G61" s="2"/>
+        <v>2.8157999999999999</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G61" s="2">
+        <v>35.92</v>
+      </c>
       <c r="H61" s="2">
-        <v>0.61642810000000003</v>
-      </c>
-      <c r="I61" s="2">
-        <v>-0.28648279999999998</v>
+        <v>1.0352460000000001</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="2" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C62" s="2" t="s">
         <v>4</v>
@@ -2452,19 +2428,19 @@
         <v>91</v>
       </c>
       <c r="E62" s="2">
-        <v>1.7956000000000001</v>
+        <v>1.7273000000000001</v>
       </c>
       <c r="F62" s="2">
-        <v>0.92420000000000002</v>
+        <v>0.60680000000000001</v>
       </c>
       <c r="G62" s="2">
-        <v>8.56</v>
+        <v>8.16</v>
       </c>
       <c r="H62" s="2">
-        <v>0.58533919999999995</v>
+        <v>0.54655949999999998</v>
       </c>
       <c r="I62" s="2">
-        <v>-7.8826800000000002E-2</v>
+        <v>-0.499556</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2472,36 +2448,34 @@
         <v>11</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D63" s="2" t="s">
         <v>91</v>
       </c>
       <c r="E63" s="2">
-        <v>3.0659999999999998</v>
+        <v>1.8523000000000001</v>
       </c>
       <c r="F63" s="2">
-        <v>2.2618999999999998</v>
-      </c>
-      <c r="G63" s="2">
-        <v>35.520000000000003</v>
-      </c>
+        <v>0.75090000000000001</v>
+      </c>
+      <c r="G63" s="2"/>
       <c r="H63" s="2">
-        <v>1.120374</v>
+        <v>0.61642810000000003</v>
       </c>
       <c r="I63" s="2">
-        <v>0.81620510000000002</v>
+        <v>-0.28648279999999998</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>4</v>
@@ -2510,27 +2484,27 @@
         <v>91</v>
       </c>
       <c r="E64" s="2">
-        <v>1.8105</v>
+        <v>1.7956000000000001</v>
       </c>
       <c r="F64" s="2">
-        <v>1.3857999999999999</v>
+        <v>0.92420000000000002</v>
       </c>
       <c r="G64" s="2">
-        <v>11.18</v>
+        <v>8.56</v>
       </c>
       <c r="H64" s="2">
-        <v>0.59360310000000005</v>
+        <v>0.58533919999999995</v>
       </c>
       <c r="I64" s="2">
-        <v>0.3262776</v>
+        <v>-7.8826800000000002E-2</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C65" s="2" t="s">
         <v>3</v>
@@ -2539,69 +2513,127 @@
         <v>91</v>
       </c>
       <c r="E65" s="2">
+        <v>3.0659999999999998</v>
+      </c>
+      <c r="F65" s="2">
+        <v>2.2618999999999998</v>
+      </c>
+      <c r="G65" s="2">
+        <v>35.520000000000003</v>
+      </c>
+      <c r="H65" s="2">
+        <v>1.120374</v>
+      </c>
+      <c r="I65" s="2">
+        <v>0.81620510000000002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="2">
+        <v>1.8105</v>
+      </c>
+      <c r="F66" s="2">
+        <v>1.3857999999999999</v>
+      </c>
+      <c r="G66" s="2">
+        <v>11.18</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0.59360310000000005</v>
+      </c>
+      <c r="I66" s="2">
+        <v>0.3262776</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E67" s="2">
         <v>3.6206999999999998</v>
       </c>
-      <c r="F65" s="2">
+      <c r="F67" s="2">
         <v>2.0116999999999998</v>
       </c>
-      <c r="G65" s="2">
+      <c r="G67" s="2">
         <v>30.33</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H67" s="2">
         <v>1.286667</v>
       </c>
-      <c r="I65" s="2">
+      <c r="I67" s="2">
         <v>0.69898009999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:9">
-      <c r="B68" s="5" t="s">
+    <row r="70" spans="1:9">
+      <c r="B70" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-    </row>
-    <row r="71" spans="1:9">
-      <c r="C71" s="4" t="s">
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+      <c r="E70" s="5"/>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="C73" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-    </row>
-    <row r="72" spans="1:9">
-      <c r="C72" s="3" t="s">
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="C74" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D72" s="3" t="s">
+      <c r="D74" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
-      <c r="G72" s="3"/>
-    </row>
-    <row r="73" spans="1:9">
-      <c r="C73" s="3" t="s">
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="C75" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D73" s="3" t="s">
+      <c r="D75" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-    </row>
-    <row r="74" spans="1:9">
-      <c r="C74" s="6"/>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6"/>
-      <c r="F74" s="6"/>
-      <c r="G74" s="6"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>